<commit_message>
Se añaden metricas pasa Nreinas
</commit_message>
<xml_diff>
--- a/AlgoritmosRecursivos/Metricas.xlsx
+++ b/AlgoritmosRecursivos/Metricas.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Torre Hanoi" sheetId="1" r:id="rId1"/>
+    <sheet name="N Reinas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Tiempo</t>
   </si>
@@ -63,7 +64,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -86,11 +87,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -98,6 +138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,7 +240,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$1</c:f>
+              <c:f>'Torre Hanoi'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -219,7 +263,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$42</c:f>
+              <c:f>'Torre Hanoi'!$A$2:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -351,7 +395,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$42</c:f>
+              <c:f>'Torre Hanoi'!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -652,7 +696,499 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'N Reinas'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tiempo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'N Reinas'!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'N Reinas'!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9999999999999997E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5999999999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8099999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0699999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4600000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.84E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.26E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.6100000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1998E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.722E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.3710999999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9065999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.3408000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8601999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25427</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1210100000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5261499999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9027300000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68839700000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.5483799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.76272700000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.92758700000000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.5489800000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.51241</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>141.23099999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34.182000000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>242.935</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>410.166</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7145.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8B1-41CF-80E7-C6E8842D42A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="362828287"/>
+        <c:axId val="377306191"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="362828287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377306191"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="377306191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362828287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1208,6 +1744,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1226,6 +2278,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1508,7 +2595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -1874,4 +2961,280 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5.5999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.8099999999999999E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.0699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.4600000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.84E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.26E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.6100000000000002E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.1998E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
+        <v>9.722E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8.3710999999999994E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.9065999999999997E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.3408000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.8601999999999998E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.25427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.1210100000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.5261499999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3.9027300000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.68839700000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <v>8.5483799999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.76272700000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.92758700000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6.5489800000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3.51241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2">
+        <v>141.23099999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2">
+        <v>34.182000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2">
+        <v>242.935</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2">
+        <v>410.166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>34</v>
+      </c>
+      <c r="B32" s="6">
+        <v>7145.59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nombre y code Metricas
</commit_message>
<xml_diff>
--- a/AlgoritmosRecursivos/Metricas.xlsx
+++ b/AlgoritmosRecursivos/Metricas.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD6D800-2DE9-4701-97A1-89D62F1670A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Torre Hanoi" sheetId="1" r:id="rId1"/>
@@ -28,13 +29,13 @@
     <t>N</t>
   </si>
   <si>
-    <t>Integrantes: Camilo Andres Garcia Zambrano(20201020047) - Miguel Veloza()</t>
+    <t>Integrantes: Camilo Andres Garcia Zambrano(20201020047) - Miguel Angel Veloza Ortiz(20192020012)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,13 +136,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,7 +163,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -199,7 +200,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -699,7 +699,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -711,7 +711,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2277,7 +2276,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2312,7 +2317,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2592,11 +2603,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,12 +2622,12 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -2625,10 +2636,10 @@
       <c r="B2" s="2">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2637,10 +2648,10 @@
       <c r="B3" s="2">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -2964,10 +2975,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -3222,16 +3233,16 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>34</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>7145.59</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>